<commit_message>
Adding timing data for Mod and Mul: Remaining are Mux, Shr and Shl
</commit_message>
<xml_diff>
--- a/TimingResults.xlsx
+++ b/TimingResults.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="14355" windowHeight="8010" firstSheet="26" activeTab="34"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="14355" windowHeight="8010" firstSheet="38" activeTab="44"/>
   </bookViews>
   <sheets>
     <sheet name="Reg2" sheetId="2" r:id="rId1"/>
@@ -42,13 +42,24 @@
     <sheet name="Inc16" sheetId="33" r:id="rId33"/>
     <sheet name="Inc32" sheetId="34" r:id="rId34"/>
     <sheet name="Inc64" sheetId="35" r:id="rId35"/>
+    <sheet name="Mod2" sheetId="36" r:id="rId36"/>
+    <sheet name="Mod8" sheetId="37" r:id="rId37"/>
+    <sheet name="Mod16" sheetId="38" r:id="rId38"/>
+    <sheet name="Mod32" sheetId="39" r:id="rId39"/>
+    <sheet name="Mod64" sheetId="40" r:id="rId40"/>
+    <sheet name="Mul2" sheetId="41" r:id="rId41"/>
+    <sheet name="Mul8" sheetId="42" r:id="rId42"/>
+    <sheet name="Mul16" sheetId="43" r:id="rId43"/>
+    <sheet name="Mul32" sheetId="44" r:id="rId44"/>
+    <sheet name="Mul64" sheetId="45" r:id="rId45"/>
+    <sheet name="Mux2" sheetId="46" r:id="rId46"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1999" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2609" uniqueCount="314">
   <si>
     <t>Name</t>
   </si>
@@ -768,6 +779,228 @@
   </si>
   <si>
     <t>D[50]</t>
+  </si>
+  <si>
+    <t>REM[1]</t>
+  </si>
+  <si>
+    <t>REM[0]</t>
+  </si>
+  <si>
+    <t>REM[6]</t>
+  </si>
+  <si>
+    <t>REM[5]</t>
+  </si>
+  <si>
+    <t>REM[7]</t>
+  </si>
+  <si>
+    <t>REM[4]</t>
+  </si>
+  <si>
+    <t>REM[3]</t>
+  </si>
+  <si>
+    <t>REM[2]</t>
+  </si>
+  <si>
+    <t>B[5]</t>
+  </si>
+  <si>
+    <t>REM[12]</t>
+  </si>
+  <si>
+    <t>REM[13]</t>
+  </si>
+  <si>
+    <t>REM[14]</t>
+  </si>
+  <si>
+    <t>REM[10]</t>
+  </si>
+  <si>
+    <t>REM[15]</t>
+  </si>
+  <si>
+    <t>REM[8]</t>
+  </si>
+  <si>
+    <t>REM[11]</t>
+  </si>
+  <si>
+    <t>REM[9]</t>
+  </si>
+  <si>
+    <t>A[31]</t>
+  </si>
+  <si>
+    <t>REM[29]</t>
+  </si>
+  <si>
+    <t>REM[30]</t>
+  </si>
+  <si>
+    <t>REM[31]</t>
+  </si>
+  <si>
+    <t>REM[26]</t>
+  </si>
+  <si>
+    <t>REM[22]</t>
+  </si>
+  <si>
+    <t>REM[27]</t>
+  </si>
+  <si>
+    <t>REM[25]</t>
+  </si>
+  <si>
+    <t>REM[28]</t>
+  </si>
+  <si>
+    <t>B[54]</t>
+  </si>
+  <si>
+    <t>REM[63]</t>
+  </si>
+  <si>
+    <t>REM[62]</t>
+  </si>
+  <si>
+    <t>REM[55]</t>
+  </si>
+  <si>
+    <t>REM[59]</t>
+  </si>
+  <si>
+    <t>REM[60]</t>
+  </si>
+  <si>
+    <t>REM[56]</t>
+  </si>
+  <si>
+    <t>REM[38]</t>
+  </si>
+  <si>
+    <t>REM[61]</t>
+  </si>
+  <si>
+    <t>REM[39]</t>
+  </si>
+  <si>
+    <t>REM[58]</t>
+  </si>
+  <si>
+    <t>PROD[1]</t>
+  </si>
+  <si>
+    <t>PROD[0]</t>
+  </si>
+  <si>
+    <t>PROD[7]</t>
+  </si>
+  <si>
+    <t>PROD[6]</t>
+  </si>
+  <si>
+    <t>PROD[5]</t>
+  </si>
+  <si>
+    <t>PROD[4]</t>
+  </si>
+  <si>
+    <t>PROD[3]</t>
+  </si>
+  <si>
+    <t>PROD[2]</t>
+  </si>
+  <si>
+    <t>PROD[15]</t>
+  </si>
+  <si>
+    <t>PROD[14]</t>
+  </si>
+  <si>
+    <t>PROD[9]</t>
+  </si>
+  <si>
+    <t>PROD[12]</t>
+  </si>
+  <si>
+    <t>PROD[11]</t>
+  </si>
+  <si>
+    <t>PROD[13]</t>
+  </si>
+  <si>
+    <t>PROD[10]</t>
+  </si>
+  <si>
+    <t>PROD[31]</t>
+  </si>
+  <si>
+    <t>PROD[29]</t>
+  </si>
+  <si>
+    <t>PROD[25]</t>
+  </si>
+  <si>
+    <t>PROD[28]</t>
+  </si>
+  <si>
+    <t>PROD[24]</t>
+  </si>
+  <si>
+    <t>PROD[27]</t>
+  </si>
+  <si>
+    <t>PROD[21]</t>
+  </si>
+  <si>
+    <t>PROD[23]</t>
+  </si>
+  <si>
+    <t>PROD[30]</t>
+  </si>
+  <si>
+    <t>PROD[20]</t>
+  </si>
+  <si>
+    <t>B[10]</t>
+  </si>
+  <si>
+    <t>PROD[63]</t>
+  </si>
+  <si>
+    <t>PROD[61]</t>
+  </si>
+  <si>
+    <t>PROD[58]</t>
+  </si>
+  <si>
+    <t>PROD[59]</t>
+  </si>
+  <si>
+    <t>PROD[57]</t>
+  </si>
+  <si>
+    <t>A[50]</t>
+  </si>
+  <si>
+    <t>PROD[55]</t>
+  </si>
+  <si>
+    <t>PROD[62]</t>
+  </si>
+  <si>
+    <t>PROD[54]</t>
+  </si>
+  <si>
+    <t>PROD[56]</t>
+  </si>
+  <si>
+    <t>PROD[60]</t>
   </si>
 </sst>
 </file>
@@ -10931,7 +11164,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
@@ -11374,6 +11607,1460 @@
       </c>
       <c r="I11" s="2">
         <v>6.9362220764160156</v>
+      </c>
+      <c r="J11" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:M3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C2" s="3">
+        <v>3</v>
+      </c>
+      <c r="D2" s="3">
+        <v>2</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="G2" s="2">
+        <v>7.2194728851318359</v>
+      </c>
+      <c r="H2" s="2">
+        <v>3.9723589420318604</v>
+      </c>
+      <c r="I2" s="2">
+        <v>3.2471139430999756</v>
+      </c>
+      <c r="J2" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C3" s="3">
+        <v>3</v>
+      </c>
+      <c r="D3" s="3">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="G3" s="2">
+        <v>6.8509516716003418</v>
+      </c>
+      <c r="H3" s="2">
+        <v>3.7599821090698242</v>
+      </c>
+      <c r="I3" s="2">
+        <v>3.0909698009490967</v>
+      </c>
+      <c r="J3" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:M9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C2" s="3">
+        <v>30</v>
+      </c>
+      <c r="D2" s="3">
+        <v>18</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="G2" s="2">
+        <v>26.44770622253418</v>
+      </c>
+      <c r="H2" s="2">
+        <v>11.953720092773438</v>
+      </c>
+      <c r="I2" s="2">
+        <v>14.493988037109375</v>
+      </c>
+      <c r="J2" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C3" s="3">
+        <v>30</v>
+      </c>
+      <c r="D3" s="3">
+        <v>18</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="G3" s="2">
+        <v>26.351524353027344</v>
+      </c>
+      <c r="H3" s="2">
+        <v>11.943933486938477</v>
+      </c>
+      <c r="I3" s="2">
+        <v>14.407594680786133</v>
+      </c>
+      <c r="J3" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C4" s="3">
+        <v>30</v>
+      </c>
+      <c r="D4" s="3">
+        <v>18</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="G4" s="2">
+        <v>26.048732757568359</v>
+      </c>
+      <c r="H4" s="2">
+        <v>11.922013282775879</v>
+      </c>
+      <c r="I4" s="2">
+        <v>14.126721382141113</v>
+      </c>
+      <c r="J4" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C5" s="3">
+        <v>29</v>
+      </c>
+      <c r="D5" s="3">
+        <v>18</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="G5" s="2">
+        <v>25.789810180664063</v>
+      </c>
+      <c r="H5" s="2">
+        <v>11.816548347473145</v>
+      </c>
+      <c r="I5" s="2">
+        <v>13.973260879516602</v>
+      </c>
+      <c r="J5" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C6" s="3">
+        <v>29</v>
+      </c>
+      <c r="D6" s="3">
+        <v>18</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="G6" s="2">
+        <v>25.567262649536133</v>
+      </c>
+      <c r="H6" s="2">
+        <v>11.812657356262207</v>
+      </c>
+      <c r="I6" s="2">
+        <v>13.754608154296875</v>
+      </c>
+      <c r="J6" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C7" s="3">
+        <v>29</v>
+      </c>
+      <c r="D7" s="3">
+        <v>18</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="G7" s="2">
+        <v>25.329374313354492</v>
+      </c>
+      <c r="H7" s="2">
+        <v>11.777127265930176</v>
+      </c>
+      <c r="I7" s="2">
+        <v>13.552247047424316</v>
+      </c>
+      <c r="J7" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C8" s="3">
+        <v>30</v>
+      </c>
+      <c r="D8" s="3">
+        <v>18</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="G8" s="2">
+        <v>25.201217651367188</v>
+      </c>
+      <c r="H8" s="2">
+        <v>12.115786552429199</v>
+      </c>
+      <c r="I8" s="2">
+        <v>13.085431098937988</v>
+      </c>
+      <c r="J8" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C9" s="3">
+        <v>30</v>
+      </c>
+      <c r="D9" s="3">
+        <v>18</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="G9" s="2">
+        <v>24.974021911621094</v>
+      </c>
+      <c r="H9" s="2">
+        <v>11.930393218994141</v>
+      </c>
+      <c r="I9" s="2">
+        <v>13.043628692626953</v>
+      </c>
+      <c r="J9" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:M11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C2" s="3">
+        <v>97</v>
+      </c>
+      <c r="D2" s="3">
+        <v>23</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="G2" s="2">
+        <v>55.800384521484375</v>
+      </c>
+      <c r="H2" s="2">
+        <v>25.739910125732422</v>
+      </c>
+      <c r="I2" s="2">
+        <v>30.060459136962891</v>
+      </c>
+      <c r="J2" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C3" s="3">
+        <v>94</v>
+      </c>
+      <c r="D3" s="3">
+        <v>23</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="G3" s="2">
+        <v>55.723297119140625</v>
+      </c>
+      <c r="H3" s="2">
+        <v>25.154022216796875</v>
+      </c>
+      <c r="I3" s="2">
+        <v>30.569253921508789</v>
+      </c>
+      <c r="J3" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C4" s="3">
+        <v>95</v>
+      </c>
+      <c r="D4" s="3">
+        <v>23</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="G4" s="2">
+        <v>55.663311004638672</v>
+      </c>
+      <c r="H4" s="2">
+        <v>25.358327865600586</v>
+      </c>
+      <c r="I4" s="2">
+        <v>30.304960250854492</v>
+      </c>
+      <c r="J4" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C5" s="3">
+        <v>95</v>
+      </c>
+      <c r="D5" s="3">
+        <v>23</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="G5" s="2">
+        <v>55.657379150390625</v>
+      </c>
+      <c r="H5" s="2">
+        <v>25.368827819824219</v>
+      </c>
+      <c r="I5" s="2">
+        <v>30.288528442382813</v>
+      </c>
+      <c r="J5" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C6" s="3">
+        <v>95</v>
+      </c>
+      <c r="D6" s="3">
+        <v>23</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="G6" s="2">
+        <v>55.634346008300781</v>
+      </c>
+      <c r="H6" s="2">
+        <v>25.346107482910156</v>
+      </c>
+      <c r="I6" s="2">
+        <v>30.288215637207031</v>
+      </c>
+      <c r="J6" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C7" s="3">
+        <v>95</v>
+      </c>
+      <c r="D7" s="3">
+        <v>23</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="G7" s="2">
+        <v>55.560489654541016</v>
+      </c>
+      <c r="H7" s="2">
+        <v>25.353948593139648</v>
+      </c>
+      <c r="I7" s="2">
+        <v>30.206518173217773</v>
+      </c>
+      <c r="J7" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C8" s="3">
+        <v>94</v>
+      </c>
+      <c r="D8" s="3">
+        <v>23</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="G8" s="2">
+        <v>55.308280944824219</v>
+      </c>
+      <c r="H8" s="2">
+        <v>25.161931991577148</v>
+      </c>
+      <c r="I8" s="2">
+        <v>30.146327972412109</v>
+      </c>
+      <c r="J8" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C9" s="3">
+        <v>94</v>
+      </c>
+      <c r="D9" s="3">
+        <v>23</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="G9" s="2">
+        <v>55.30511474609375</v>
+      </c>
+      <c r="H9" s="2">
+        <v>24.931049346923828</v>
+      </c>
+      <c r="I9" s="2">
+        <v>30.374050140380859</v>
+      </c>
+      <c r="J9" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C10" s="3">
+        <v>95</v>
+      </c>
+      <c r="D10" s="3">
+        <v>23</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="G10" s="2">
+        <v>55.184833526611328</v>
+      </c>
+      <c r="H10" s="2">
+        <v>25.372549057006836</v>
+      </c>
+      <c r="I10" s="2">
+        <v>29.812267303466797</v>
+      </c>
+      <c r="J10" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C11" s="3">
+        <v>94</v>
+      </c>
+      <c r="D11" s="3">
+        <v>23</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="G11" s="2">
+        <v>54.975639343261719</v>
+      </c>
+      <c r="H11" s="2">
+        <v>24.931999206542969</v>
+      </c>
+      <c r="I11" s="2">
+        <v>30.043622970581055</v>
+      </c>
+      <c r="J11" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:M11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C2" s="3">
+        <v>321</v>
+      </c>
+      <c r="D2" s="3">
+        <v>35</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="G2" s="2">
+        <v>137.19462585449219</v>
+      </c>
+      <c r="H2" s="2">
+        <v>60.605358123779297</v>
+      </c>
+      <c r="I2" s="2">
+        <v>76.5892333984375</v>
+      </c>
+      <c r="J2" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C3" s="3">
+        <v>321</v>
+      </c>
+      <c r="D3" s="3">
+        <v>35</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="G3" s="2">
+        <v>137.18397521972656</v>
+      </c>
+      <c r="H3" s="2">
+        <v>60.584030151367188</v>
+      </c>
+      <c r="I3" s="2">
+        <v>76.59991455078125</v>
+      </c>
+      <c r="J3" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C4" s="3">
+        <v>321</v>
+      </c>
+      <c r="D4" s="3">
+        <v>35</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="G4" s="2">
+        <v>136.84002685546875</v>
+      </c>
+      <c r="H4" s="2">
+        <v>60.598644256591797</v>
+      </c>
+      <c r="I4" s="2">
+        <v>76.241363525390625</v>
+      </c>
+      <c r="J4" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C5" s="3">
+        <v>317</v>
+      </c>
+      <c r="D5" s="3">
+        <v>35</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="G5" s="2">
+        <v>136.83119201660156</v>
+      </c>
+      <c r="H5" s="2">
+        <v>60.142875671386719</v>
+      </c>
+      <c r="I5" s="2">
+        <v>76.688240051269531</v>
+      </c>
+      <c r="J5" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C6" s="3">
+        <v>317</v>
+      </c>
+      <c r="D6" s="3">
+        <v>35</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="G6" s="2">
+        <v>136.7430419921875</v>
+      </c>
+      <c r="H6" s="2">
+        <v>60.168319702148438</v>
+      </c>
+      <c r="I6" s="2">
+        <v>76.574661254882813</v>
+      </c>
+      <c r="J6" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C7" s="3">
+        <v>317</v>
+      </c>
+      <c r="D7" s="3">
+        <v>35</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="G7" s="2">
+        <v>136.61900329589844</v>
+      </c>
+      <c r="H7" s="2">
+        <v>60.884319305419922</v>
+      </c>
+      <c r="I7" s="2">
+        <v>75.734649658203125</v>
+      </c>
+      <c r="J7" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C8" s="3">
+        <v>317</v>
+      </c>
+      <c r="D8" s="3">
+        <v>35</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="G8" s="2">
+        <v>136.59274291992187</v>
+      </c>
+      <c r="H8" s="2">
+        <v>60.390869140625</v>
+      </c>
+      <c r="I8" s="2">
+        <v>76.201820373535156</v>
+      </c>
+      <c r="J8" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C9" s="3">
+        <v>317</v>
+      </c>
+      <c r="D9" s="3">
+        <v>35</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="G9" s="2">
+        <v>136.46539306640625</v>
+      </c>
+      <c r="H9" s="2">
+        <v>60.145622253417969</v>
+      </c>
+      <c r="I9" s="2">
+        <v>76.319694519042969</v>
+      </c>
+      <c r="J9" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C10" s="3">
+        <v>317</v>
+      </c>
+      <c r="D10" s="3">
+        <v>35</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="G10" s="2">
+        <v>136.45466613769531</v>
+      </c>
+      <c r="H10" s="2">
+        <v>60.855361938476563</v>
+      </c>
+      <c r="I10" s="2">
+        <v>75.599258422851563</v>
+      </c>
+      <c r="J10" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C11" s="3">
+        <v>320</v>
+      </c>
+      <c r="D11" s="3">
+        <v>35</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="G11" s="2">
+        <v>136.19656372070313</v>
+      </c>
+      <c r="H11" s="2">
+        <v>60.736907958984375</v>
+      </c>
+      <c r="I11" s="2">
+        <v>75.459632873535156</v>
       </c>
       <c r="J11" s="2" t="e">
         <v>#DIV/0!</v>
@@ -11826,6 +13513,2405 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:M11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C2" s="3">
+        <v>1135</v>
+      </c>
+      <c r="D2" s="3">
+        <v>69</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="G2" s="2">
+        <v>414.75662231445312</v>
+      </c>
+      <c r="H2" s="2">
+        <v>175.15606689453125</v>
+      </c>
+      <c r="I2" s="2">
+        <v>239.59913635253906</v>
+      </c>
+      <c r="J2" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C3" s="3">
+        <v>1135</v>
+      </c>
+      <c r="D3" s="3">
+        <v>69</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="G3" s="2">
+        <v>414.13348388671875</v>
+      </c>
+      <c r="H3" s="2">
+        <v>175.19886779785156</v>
+      </c>
+      <c r="I3" s="2">
+        <v>238.93321228027344</v>
+      </c>
+      <c r="J3" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1135</v>
+      </c>
+      <c r="D4" s="3">
+        <v>69</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="G4" s="2">
+        <v>413.97439575195312</v>
+      </c>
+      <c r="H4" s="2">
+        <v>175.1949462890625</v>
+      </c>
+      <c r="I4" s="2">
+        <v>238.77809143066406</v>
+      </c>
+      <c r="J4" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C5" s="3">
+        <v>1135</v>
+      </c>
+      <c r="D5" s="3">
+        <v>69</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="G5" s="2">
+        <v>413.96383666992187</v>
+      </c>
+      <c r="H5" s="2">
+        <v>175.38706970214844</v>
+      </c>
+      <c r="I5" s="2">
+        <v>238.57540893554688</v>
+      </c>
+      <c r="J5" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C6" s="3">
+        <v>1134</v>
+      </c>
+      <c r="D6" s="3">
+        <v>69</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="G6" s="2">
+        <v>413.93182373046875</v>
+      </c>
+      <c r="H6" s="2">
+        <v>175.2974853515625</v>
+      </c>
+      <c r="I6" s="2">
+        <v>238.6329345703125</v>
+      </c>
+      <c r="J6" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C7" s="3">
+        <v>1134</v>
+      </c>
+      <c r="D7" s="3">
+        <v>69</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="G7" s="2">
+        <v>413.87249755859375</v>
+      </c>
+      <c r="H7" s="2">
+        <v>175.06912231445312</v>
+      </c>
+      <c r="I7" s="2">
+        <v>238.80198669433594</v>
+      </c>
+      <c r="J7" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C8" s="3">
+        <v>1131</v>
+      </c>
+      <c r="D8" s="3">
+        <v>69</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="G8" s="2">
+        <v>413.861572265625</v>
+      </c>
+      <c r="H8" s="2">
+        <v>174.75419616699219</v>
+      </c>
+      <c r="I8" s="2">
+        <v>239.10601806640625</v>
+      </c>
+      <c r="J8" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C9" s="3">
+        <v>1135</v>
+      </c>
+      <c r="D9" s="3">
+        <v>69</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="G9" s="2">
+        <v>413.72476196289062</v>
+      </c>
+      <c r="H9" s="2">
+        <v>175.18624877929687</v>
+      </c>
+      <c r="I9" s="2">
+        <v>238.53715515136719</v>
+      </c>
+      <c r="J9" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C10" s="3">
+        <v>1131</v>
+      </c>
+      <c r="D10" s="3">
+        <v>69</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="G10" s="2">
+        <v>413.71853637695312</v>
+      </c>
+      <c r="H10" s="2">
+        <v>174.75506591796875</v>
+      </c>
+      <c r="I10" s="2">
+        <v>238.96206665039062</v>
+      </c>
+      <c r="J10" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C11" s="3">
+        <v>1135</v>
+      </c>
+      <c r="D11" s="3">
+        <v>69</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="G11" s="2">
+        <v>413.67727661132812</v>
+      </c>
+      <c r="H11" s="2">
+        <v>175.19400024414062</v>
+      </c>
+      <c r="I11" s="2">
+        <v>238.48184204101562</v>
+      </c>
+      <c r="J11" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:M3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C2" s="3">
+        <v>3</v>
+      </c>
+      <c r="D2" s="3">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="G2" s="2">
+        <v>7.2194728851318359</v>
+      </c>
+      <c r="H2" s="2">
+        <v>3.9723589420318604</v>
+      </c>
+      <c r="I2" s="2">
+        <v>3.2471139430999756</v>
+      </c>
+      <c r="J2" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C3" s="3">
+        <v>3</v>
+      </c>
+      <c r="D3" s="3">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="G3" s="2">
+        <v>6.5776233673095703</v>
+      </c>
+      <c r="H3" s="2">
+        <v>3.7190241813659668</v>
+      </c>
+      <c r="I3" s="2">
+        <v>2.8585996627807617</v>
+      </c>
+      <c r="J3" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:M9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C2" s="3">
+        <v>9</v>
+      </c>
+      <c r="D2" s="3">
+        <v>16</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="G2" s="2">
+        <v>12.175518989562988</v>
+      </c>
+      <c r="H2" s="2">
+        <v>5.7785153388977051</v>
+      </c>
+      <c r="I2" s="2">
+        <v>6.3970026969909668</v>
+      </c>
+      <c r="J2" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C3" s="3">
+        <v>8</v>
+      </c>
+      <c r="D3" s="3">
+        <v>16</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="G3" s="2">
+        <v>11.293938636779785</v>
+      </c>
+      <c r="H3" s="2">
+        <v>5.8562221527099609</v>
+      </c>
+      <c r="I3" s="2">
+        <v>5.4377155303955078</v>
+      </c>
+      <c r="J3" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C4" s="3">
+        <v>8</v>
+      </c>
+      <c r="D4" s="3">
+        <v>16</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="G4" s="2">
+        <v>11.066732406616211</v>
+      </c>
+      <c r="H4" s="2">
+        <v>5.7824358940124512</v>
+      </c>
+      <c r="I4" s="2">
+        <v>5.2842965126037598</v>
+      </c>
+      <c r="J4" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C5" s="3">
+        <v>7</v>
+      </c>
+      <c r="D5" s="3">
+        <v>16</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="G5" s="2">
+        <v>10.943323135375977</v>
+      </c>
+      <c r="H5" s="2">
+        <v>5.2560510635375977</v>
+      </c>
+      <c r="I5" s="2">
+        <v>5.6872730255126953</v>
+      </c>
+      <c r="J5" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C6" s="3">
+        <v>6</v>
+      </c>
+      <c r="D6" s="3">
+        <v>16</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="G6" s="2">
+        <v>10.066211700439453</v>
+      </c>
+      <c r="H6" s="2">
+        <v>4.6491603851318359</v>
+      </c>
+      <c r="I6" s="2">
+        <v>5.4170517921447754</v>
+      </c>
+      <c r="J6" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C7" s="3">
+        <v>4</v>
+      </c>
+      <c r="D7" s="3">
+        <v>16</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="G7" s="2">
+        <v>8.4619474411010742</v>
+      </c>
+      <c r="H7" s="2">
+        <v>4.5106287002563477</v>
+      </c>
+      <c r="I7" s="2">
+        <v>3.9513185024261475</v>
+      </c>
+      <c r="J7" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C8" s="3">
+        <v>4</v>
+      </c>
+      <c r="D8" s="3">
+        <v>16</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="G8" s="2">
+        <v>8.0479440689086914</v>
+      </c>
+      <c r="H8" s="2">
+        <v>4.1462888717651367</v>
+      </c>
+      <c r="I8" s="2">
+        <v>3.901655912399292</v>
+      </c>
+      <c r="J8" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C9" s="3">
+        <v>4</v>
+      </c>
+      <c r="D9" s="3">
+        <v>12</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="G9" s="2">
+        <v>7.697329044342041</v>
+      </c>
+      <c r="H9" s="2">
+        <v>4.1398096084594727</v>
+      </c>
+      <c r="I9" s="2">
+        <v>3.5575201511383057</v>
+      </c>
+      <c r="J9" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:M11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C2" s="3">
+        <v>3</v>
+      </c>
+      <c r="D2" s="3">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="G2" s="2">
+        <v>12.580864906311035</v>
+      </c>
+      <c r="H2" s="2">
+        <v>7.486269474029541</v>
+      </c>
+      <c r="I2" s="2">
+        <v>5.0945959091186523</v>
+      </c>
+      <c r="J2" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C3" s="3">
+        <v>3</v>
+      </c>
+      <c r="D3" s="3">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="G3" s="2">
+        <v>12.470714569091797</v>
+      </c>
+      <c r="H3" s="2">
+        <v>7.5011491775512695</v>
+      </c>
+      <c r="I3" s="2">
+        <v>4.9695653915405273</v>
+      </c>
+      <c r="J3" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C4" s="3">
+        <v>3</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="G4" s="2">
+        <v>12.443514823913574</v>
+      </c>
+      <c r="H4" s="2">
+        <v>7.4913215637207031</v>
+      </c>
+      <c r="I4" s="2">
+        <v>4.9521942138671875</v>
+      </c>
+      <c r="J4" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C5" s="3">
+        <v>3</v>
+      </c>
+      <c r="D5" s="3">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="G5" s="2">
+        <v>12.321322441101074</v>
+      </c>
+      <c r="H5" s="2">
+        <v>7.5082340240478516</v>
+      </c>
+      <c r="I5" s="2">
+        <v>4.8130879402160645</v>
+      </c>
+      <c r="J5" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C6" s="3">
+        <v>3</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="G6" s="2">
+        <v>12.30695915222168</v>
+      </c>
+      <c r="H6" s="2">
+        <v>7.5048713684082031</v>
+      </c>
+      <c r="I6" s="2">
+        <v>4.8020882606506348</v>
+      </c>
+      <c r="J6" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C7" s="3">
+        <v>3</v>
+      </c>
+      <c r="D7" s="3">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="G7" s="2">
+        <v>12.30600643157959</v>
+      </c>
+      <c r="H7" s="2">
+        <v>7.4906506538391113</v>
+      </c>
+      <c r="I7" s="2">
+        <v>4.8153562545776367</v>
+      </c>
+      <c r="J7" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C8" s="3">
+        <v>3</v>
+      </c>
+      <c r="D8" s="3">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="G8" s="2">
+        <v>12.300786018371582</v>
+      </c>
+      <c r="H8" s="2">
+        <v>7.4784302711486816</v>
+      </c>
+      <c r="I8" s="2">
+        <v>4.8223562240600586</v>
+      </c>
+      <c r="J8" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C9" s="3">
+        <v>3</v>
+      </c>
+      <c r="D9" s="3">
+        <v>1</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="G9" s="2">
+        <v>12.262669563293457</v>
+      </c>
+      <c r="H9" s="2">
+        <v>7.4853448867797852</v>
+      </c>
+      <c r="I9" s="2">
+        <v>4.7773251533508301</v>
+      </c>
+      <c r="J9" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C10" s="3">
+        <v>3</v>
+      </c>
+      <c r="D10" s="3">
+        <v>1</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="G10" s="2">
+        <v>12.261877059936523</v>
+      </c>
+      <c r="H10" s="2">
+        <v>7.493253231048584</v>
+      </c>
+      <c r="I10" s="2">
+        <v>4.7686238288879395</v>
+      </c>
+      <c r="J10" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C11" s="3">
+        <v>3</v>
+      </c>
+      <c r="D11" s="3">
+        <v>1</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="G11" s="2">
+        <v>12.26185417175293</v>
+      </c>
+      <c r="H11" s="2">
+        <v>7.4865908622741699</v>
+      </c>
+      <c r="I11" s="2">
+        <v>4.7752633094787598</v>
+      </c>
+      <c r="J11" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:M11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C2" s="3">
+        <v>7</v>
+      </c>
+      <c r="D2" s="3">
+        <v>2</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="G2" s="2">
+        <v>18.898551940917969</v>
+      </c>
+      <c r="H2" s="2">
+        <v>10.326019287109375</v>
+      </c>
+      <c r="I2" s="2">
+        <v>8.5725326538085937</v>
+      </c>
+      <c r="J2" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C3" s="3">
+        <v>7</v>
+      </c>
+      <c r="D3" s="3">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="G3" s="2">
+        <v>18.77619743347168</v>
+      </c>
+      <c r="H3" s="2">
+        <v>10.350733757019043</v>
+      </c>
+      <c r="I3" s="2">
+        <v>8.4254646301269531</v>
+      </c>
+      <c r="J3" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C4" s="3">
+        <v>8</v>
+      </c>
+      <c r="D4" s="3">
+        <v>2</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="G4" s="2">
+        <v>18.626838684082031</v>
+      </c>
+      <c r="H4" s="2">
+        <v>10.317008972167969</v>
+      </c>
+      <c r="I4" s="2">
+        <v>8.3098297119140625</v>
+      </c>
+      <c r="J4" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C5" s="3">
+        <v>7</v>
+      </c>
+      <c r="D5" s="3">
+        <v>2</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="G5" s="2">
+        <v>18.538715362548828</v>
+      </c>
+      <c r="H5" s="2">
+        <v>10.254290580749512</v>
+      </c>
+      <c r="I5" s="2">
+        <v>8.2844219207763672</v>
+      </c>
+      <c r="J5" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C6" s="3">
+        <v>8</v>
+      </c>
+      <c r="D6" s="3">
+        <v>2</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="G6" s="2">
+        <v>18.452905654907227</v>
+      </c>
+      <c r="H6" s="2">
+        <v>10.217790603637695</v>
+      </c>
+      <c r="I6" s="2">
+        <v>8.2351140975952148</v>
+      </c>
+      <c r="J6" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C7" s="3">
+        <v>8</v>
+      </c>
+      <c r="D7" s="3">
+        <v>2</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="G7" s="2">
+        <v>18.44514274597168</v>
+      </c>
+      <c r="H7" s="2">
+        <v>10.314252853393555</v>
+      </c>
+      <c r="I7" s="2">
+        <v>8.1308879852294922</v>
+      </c>
+      <c r="J7" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C8" s="3">
+        <v>7</v>
+      </c>
+      <c r="D8" s="3">
+        <v>2</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="G8" s="2">
+        <v>18.291835784912109</v>
+      </c>
+      <c r="H8" s="2">
+        <v>10.223246574401855</v>
+      </c>
+      <c r="I8" s="2">
+        <v>8.0685853958129883</v>
+      </c>
+      <c r="J8" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C9" s="3">
+        <v>7</v>
+      </c>
+      <c r="D9" s="3">
+        <v>2</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="G9" s="2">
+        <v>18.260360717773437</v>
+      </c>
+      <c r="H9" s="2">
+        <v>10.202704429626465</v>
+      </c>
+      <c r="I9" s="2">
+        <v>8.0576543807983398</v>
+      </c>
+      <c r="J9" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C10" s="3">
+        <v>7</v>
+      </c>
+      <c r="D10" s="3">
+        <v>2</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="G10" s="2">
+        <v>18.077140808105469</v>
+      </c>
+      <c r="H10" s="2">
+        <v>10.233407020568848</v>
+      </c>
+      <c r="I10" s="2">
+        <v>7.8437337875366211</v>
+      </c>
+      <c r="J10" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C11" s="3">
+        <v>7</v>
+      </c>
+      <c r="D11" s="3">
+        <v>2</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="G11" s="2">
+        <v>18.052396774291992</v>
+      </c>
+      <c r="H11" s="2">
+        <v>10.119762420654297</v>
+      </c>
+      <c r="I11" s="2">
+        <v>7.9326333999633789</v>
+      </c>
+      <c r="J11" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:M11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C2" s="3">
+        <v>9</v>
+      </c>
+      <c r="D2" s="3">
+        <v>4</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="G2" s="2">
+        <v>23.582874298095703</v>
+      </c>
+      <c r="H2" s="2">
+        <v>13.747920036315918</v>
+      </c>
+      <c r="I2" s="2">
+        <v>9.8349523544311523</v>
+      </c>
+      <c r="J2" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C3" s="3">
+        <v>11</v>
+      </c>
+      <c r="D3" s="3">
+        <v>4</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="G3" s="2">
+        <v>23.370506286621094</v>
+      </c>
+      <c r="H3" s="2">
+        <v>13.936098098754883</v>
+      </c>
+      <c r="I3" s="2">
+        <v>9.4344091415405273</v>
+      </c>
+      <c r="J3" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C4" s="3">
+        <v>10</v>
+      </c>
+      <c r="D4" s="3">
+        <v>4</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="G4" s="2">
+        <v>23.299083709716797</v>
+      </c>
+      <c r="H4" s="2">
+        <v>13.944863319396973</v>
+      </c>
+      <c r="I4" s="2">
+        <v>9.354222297668457</v>
+      </c>
+      <c r="J4" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C5" s="3">
+        <v>10</v>
+      </c>
+      <c r="D5" s="3">
+        <v>4</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="G5" s="2">
+        <v>23.232326507568359</v>
+      </c>
+      <c r="H5" s="2">
+        <v>13.845925331115723</v>
+      </c>
+      <c r="I5" s="2">
+        <v>9.3864021301269531</v>
+      </c>
+      <c r="J5" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C6" s="3">
+        <v>10</v>
+      </c>
+      <c r="D6" s="3">
+        <v>4</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="G6" s="2">
+        <v>23.189847946166992</v>
+      </c>
+      <c r="H6" s="2">
+        <v>13.839748382568359</v>
+      </c>
+      <c r="I6" s="2">
+        <v>9.3501005172729492</v>
+      </c>
+      <c r="J6" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C7" s="3">
+        <v>8</v>
+      </c>
+      <c r="D7" s="3">
+        <v>2</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="G7" s="2">
+        <v>23.117448806762695</v>
+      </c>
+      <c r="H7" s="2">
+        <v>12.166938781738281</v>
+      </c>
+      <c r="I7" s="2">
+        <v>10.950510025024414</v>
+      </c>
+      <c r="J7" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C8" s="3">
+        <v>11</v>
+      </c>
+      <c r="D8" s="3">
+        <v>4</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="G8" s="2">
+        <v>23.056329727172852</v>
+      </c>
+      <c r="H8" s="2">
+        <v>14.063728332519531</v>
+      </c>
+      <c r="I8" s="2">
+        <v>8.9926061630249023</v>
+      </c>
+      <c r="J8" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C9" s="3">
+        <v>8</v>
+      </c>
+      <c r="D9" s="3">
+        <v>2</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="G9" s="2">
+        <v>22.737129211425781</v>
+      </c>
+      <c r="H9" s="2">
+        <v>11.81043529510498</v>
+      </c>
+      <c r="I9" s="2">
+        <v>10.926692008972168</v>
+      </c>
+      <c r="J9" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C10" s="3">
+        <v>8</v>
+      </c>
+      <c r="D10" s="3">
+        <v>2</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="G10" s="2">
+        <v>22.700201034545898</v>
+      </c>
+      <c r="H10" s="2">
+        <v>12.229127883911133</v>
+      </c>
+      <c r="I10" s="2">
+        <v>10.471073150634766</v>
+      </c>
+      <c r="J10" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C11" s="3">
+        <v>10</v>
+      </c>
+      <c r="D11" s="3">
+        <v>4</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="G11" s="2">
+        <v>22.623178482055664</v>
+      </c>
+      <c r="H11" s="2">
+        <v>13.9283447265625</v>
+      </c>
+      <c r="I11" s="2">
+        <v>8.6948356628417969</v>
+      </c>
+      <c r="J11" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L11"/>

</xml_diff>

<commit_message>
Finished up TimingResults.xlsx workbook. Made a vba script to format the last sheet nicely (latency_generator.vb). Final result ready for viewing in DCPL_LAT.txt
</commit_message>
<xml_diff>
--- a/TimingResults.xlsx
+++ b/TimingResults.xlsx
@@ -2,9 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="14355" windowHeight="8010" firstSheet="52" activeTab="59"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="14355" windowHeight="8010" firstSheet="59" activeTab="60"/>
   </bookViews>
   <sheets>
     <sheet name="Reg2" sheetId="2" r:id="rId1"/>
@@ -67,13 +67,14 @@
     <sheet name="SHR16" sheetId="58" r:id="rId58"/>
     <sheet name="SHR32" sheetId="59" r:id="rId59"/>
     <sheet name="SHR64" sheetId="60" r:id="rId60"/>
+    <sheet name="DCPL_LAT" sheetId="76" r:id="rId61"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3499" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3536" uniqueCount="348">
   <si>
     <t>Name</t>
   </si>
@@ -1081,6 +1082,42 @@
   </si>
   <si>
     <t>D[16]</t>
+  </si>
+  <si>
+    <t>REG</t>
+  </si>
+  <si>
+    <t>ADD</t>
+  </si>
+  <si>
+    <t>SUB</t>
+  </si>
+  <si>
+    <t>COMP</t>
+  </si>
+  <si>
+    <t>DEC</t>
+  </si>
+  <si>
+    <t>DIV</t>
+  </si>
+  <si>
+    <t>INC</t>
+  </si>
+  <si>
+    <t>MOD</t>
+  </si>
+  <si>
+    <t>MUL</t>
+  </si>
+  <si>
+    <t>MUX2x1</t>
+  </si>
+  <si>
+    <t>SHL</t>
+  </si>
+  <si>
+    <t>SHR</t>
   </si>
 </sst>
 </file>
@@ -1433,10 +1470,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:M7"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1735,6 +1773,7 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2201,6 +2240,7 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2339,6 +2379,7 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2723,6 +2764,7 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet13"/>
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3189,6 +3231,7 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet14"/>
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3655,6 +3698,7 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet15"/>
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4121,6 +4165,7 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet16"/>
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4300,6 +4345,7 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet17"/>
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4479,6 +4525,7 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet18"/>
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4658,6 +4705,7 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet19"/>
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4837,6 +4885,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5303,6 +5352,7 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet20"/>
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5482,6 +5532,7 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet21"/>
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5620,6 +5671,7 @@
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet22"/>
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6004,6 +6056,7 @@
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet23"/>
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6470,6 +6523,7 @@
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet24"/>
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6936,6 +6990,7 @@
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet25"/>
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7402,6 +7457,7 @@
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet26"/>
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7540,6 +7596,7 @@
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet27"/>
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7924,6 +7981,7 @@
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet28"/>
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8390,6 +8448,7 @@
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet29"/>
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8856,6 +8915,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9322,6 +9382,7 @@
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet30"/>
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9788,6 +9849,7 @@
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet31"/>
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9926,6 +9988,7 @@
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet32"/>
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10310,6 +10373,7 @@
 
 <file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet33"/>
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10776,6 +10840,7 @@
 
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet34"/>
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11242,6 +11307,7 @@
 
 <file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet35"/>
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11708,6 +11774,7 @@
 
 <file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet36"/>
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11846,6 +11913,7 @@
 
 <file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet37"/>
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12230,6 +12298,7 @@
 
 <file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet38"/>
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12696,6 +12765,7 @@
 
 <file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet39"/>
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -13162,6 +13232,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -13595,6 +13666,7 @@
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet40"/>
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -14061,6 +14133,7 @@
 
 <file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet41"/>
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -14199,6 +14272,7 @@
 
 <file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet42"/>
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -14583,6 +14657,7 @@
 
 <file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet43"/>
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -15049,6 +15124,7 @@
 
 <file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet44"/>
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -15515,6 +15591,7 @@
 
 <file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet45"/>
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -15982,6 +16059,7 @@
 
 <file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet46"/>
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -16120,6 +16198,7 @@
 
 <file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet47"/>
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -16504,6 +16583,7 @@
 
 <file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet48"/>
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -16970,6 +17050,7 @@
 
 <file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet49"/>
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -17436,6 +17517,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -17869,6 +17951,7 @@
 
 <file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet50"/>
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -18335,18 +18418,147 @@
 
 <file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <sheetPr codeName="Sheet51"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C2" s="3">
+        <v>3</v>
+      </c>
+      <c r="D2" s="3">
+        <v>2</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G2" s="2">
+        <v>7.2194728851318359</v>
+      </c>
+      <c r="H2" s="2">
+        <v>3.9723589420318604</v>
+      </c>
+      <c r="I2" s="2">
+        <v>3.2471139430999756</v>
+      </c>
+      <c r="J2" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C3" s="3">
+        <v>3</v>
+      </c>
+      <c r="D3" s="3">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G3" s="2">
+        <v>6.8509516716003418</v>
+      </c>
+      <c r="H3" s="2">
+        <v>3.7599821090698242</v>
+      </c>
+      <c r="I3" s="2">
+        <v>3.0909698009490967</v>
+      </c>
+      <c r="J3" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet52"/>
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -18731,6 +18943,7 @@
 
 <file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet53"/>
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -19197,6 +19410,7 @@
 
 <file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet54"/>
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -19663,6 +19877,7 @@
 
 <file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet55"/>
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -20129,6 +20344,7 @@
 
 <file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet56"/>
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -20267,6 +20483,7 @@
 
 <file path=xl/worksheets/sheet57.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet57"/>
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -20651,6 +20868,7 @@
 
 <file path=xl/worksheets/sheet58.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet58"/>
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -21117,6 +21335,7 @@
 
 <file path=xl/worksheets/sheet59.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet59"/>
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -21583,6 +21802,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -21721,9 +21941,10 @@
 
 <file path=xl/worksheets/sheet60.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet60"/>
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:M11"/>
     </sheetView>
   </sheetViews>
@@ -22186,8 +22407,265 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet61.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet76"/>
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>336</v>
+      </c>
+      <c r="B1">
+        <v>4.9208202362060547</v>
+      </c>
+      <c r="C1">
+        <v>5.1751894950866699</v>
+      </c>
+      <c r="D1">
+        <v>5.4370088577270508</v>
+      </c>
+      <c r="E1">
+        <v>6.5318489074707031</v>
+      </c>
+      <c r="F1">
+        <v>7.4555063247680664</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>337</v>
+      </c>
+      <c r="B2">
+        <v>6.8849177360534668</v>
+      </c>
+      <c r="C2">
+        <v>8.6643447875976562</v>
+      </c>
+      <c r="D2">
+        <v>9.7914276123046875</v>
+      </c>
+      <c r="E2">
+        <v>12.549606323242188</v>
+      </c>
+      <c r="F2">
+        <v>13.581467628479004</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>338</v>
+      </c>
+      <c r="B3">
+        <v>7.2194728851318359</v>
+      </c>
+      <c r="C3">
+        <v>8.6643447875976562</v>
+      </c>
+      <c r="D3">
+        <v>9.7914276123046875</v>
+      </c>
+      <c r="E3">
+        <v>12.549606323242188</v>
+      </c>
+      <c r="F3">
+        <v>13.581467628479004</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>339</v>
+      </c>
+      <c r="B4">
+        <v>7.1687474250793457</v>
+      </c>
+      <c r="C4">
+        <v>9.4029655456542969</v>
+      </c>
+      <c r="D4">
+        <v>10.20001220703125</v>
+      </c>
+      <c r="E4">
+        <v>10.392529487609863</v>
+      </c>
+      <c r="F4">
+        <v>11.818764686584473</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>340</v>
+      </c>
+      <c r="B5">
+        <v>6.6915583610534668</v>
+      </c>
+      <c r="C5">
+        <v>7.9896674156188965</v>
+      </c>
+      <c r="D5">
+        <v>9.3042325973510742</v>
+      </c>
+      <c r="E5">
+        <v>11.017780303955078</v>
+      </c>
+      <c r="F5">
+        <v>14.229767799377441</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>341</v>
+      </c>
+      <c r="B6">
+        <v>7.0951600074768066</v>
+      </c>
+      <c r="C6">
+        <v>23.024412155151367</v>
+      </c>
+      <c r="D6">
+        <v>52.615036010742188</v>
+      </c>
+      <c r="E6">
+        <v>133.12629699707031</v>
+      </c>
+      <c r="F6">
+        <v>407.22406005859375</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>342</v>
+      </c>
+      <c r="B7">
+        <v>6.6915583610534668</v>
+      </c>
+      <c r="C7">
+        <v>8.1548032760620117</v>
+      </c>
+      <c r="D7">
+        <v>8.8057050704956055</v>
+      </c>
+      <c r="E7">
+        <v>10.888552665710449</v>
+      </c>
+      <c r="F7">
+        <v>13.675131797790527</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>343</v>
+      </c>
+      <c r="B8">
+        <v>7.2194728851318359</v>
+      </c>
+      <c r="C8">
+        <v>26.44770622253418</v>
+      </c>
+      <c r="D8">
+        <v>55.800384521484375</v>
+      </c>
+      <c r="E8">
+        <v>137.19462585449219</v>
+      </c>
+      <c r="F8">
+        <v>414.75662231445312</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>344</v>
+      </c>
+      <c r="B9">
+        <v>7.2194728851318359</v>
+      </c>
+      <c r="C9">
+        <v>12.175518989562988</v>
+      </c>
+      <c r="D9">
+        <v>12.580864906311035</v>
+      </c>
+      <c r="E9">
+        <v>18.898551940917969</v>
+      </c>
+      <c r="F9">
+        <v>23.582874298095703</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>345</v>
+      </c>
+      <c r="B10">
+        <v>7.2845816612243652</v>
+      </c>
+      <c r="C10">
+        <v>7.8291311264038086</v>
+      </c>
+      <c r="D10">
+        <v>8.8097333908081055</v>
+      </c>
+      <c r="E10">
+        <v>11.198925971984863</v>
+      </c>
+      <c r="F10">
+        <v>14.578961372375488</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>346</v>
+      </c>
+      <c r="B11">
+        <v>7.2194728851318359</v>
+      </c>
+      <c r="C11">
+        <v>8.9147806167602539</v>
+      </c>
+      <c r="D11">
+        <v>11.094443321228027</v>
+      </c>
+      <c r="E11">
+        <v>14.217499732971191</v>
+      </c>
+      <c r="F11">
+        <v>21.493843078613281</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>347</v>
+      </c>
+      <c r="B12">
+        <v>7.0951600074768066</v>
+      </c>
+      <c r="C12">
+        <v>8.768580436706543</v>
+      </c>
+      <c r="D12">
+        <v>10.817635536193848</v>
+      </c>
+      <c r="E12">
+        <v>13.373261451721191</v>
+      </c>
+      <c r="F12">
+        <v>20.366817474365234</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -22572,6 +23050,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -23038,6 +23517,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>